<commit_message>
Bunch of ajdustments to make mcts run with respawner
</commit_message>
<xml_diff>
--- a/src/generative_playground/molecules/train/pg/conditional/v2/results.xlsx
+++ b/src/generative_playground/molecules/train/pg/conditional/v2/results.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egork\Dropbox\GitHub\deep_games\generative_playground\src\generative_playground\molecules\train\pg\conditional\v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E267EEBC-CB45-48E6-AF1E-2956D16EAA20}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F786787-5E73-4AE6-B341-BD20F560E6E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{26FE2BFE-F311-4EBE-9F7C-EED9F64B980A}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="4608" windowHeight="3600" activeTab="1" xr2:uid="{26FE2BFE-F311-4EBE-9F7C-EED9F64B980A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="new run with truncated entropy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>Target number</t>
   </si>
@@ -51,6 +53,30 @@
   </si>
   <si>
     <t>Never even got a start</t>
+  </si>
+  <si>
+    <t>Tries to max out size</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Was still running</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Y?</t>
+  </si>
+  <si>
+    <t>lr = 0.05</t>
+  </si>
+  <si>
+    <t>ew = 3</t>
+  </si>
+  <si>
+    <t>Saturation at 0.3 with increasing spikes to 0.85</t>
   </si>
 </sst>
 </file>
@@ -66,12 +92,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,8 +124,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,7 +444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53E232D9-B278-4D63-94A8-DBAF1CD7EEAD}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -561,4 +601,313 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FC20DC-CE70-4625-AD9D-6C4ED40A3215}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="15.734375" customWidth="1"/>
+    <col min="2" max="2" width="10.62890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="C3" s="2">
+        <v>220</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>0.65</v>
+      </c>
+      <c r="C4" s="2">
+        <v>210</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>0.66</v>
+      </c>
+      <c r="C5" s="2">
+        <v>210</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0.76</v>
+      </c>
+      <c r="C6" s="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>0.97</v>
+      </c>
+      <c r="C7" s="2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>0.8</v>
+      </c>
+      <c r="C8" s="2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>0.84</v>
+      </c>
+      <c r="C9" s="2">
+        <v>600</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>0.92</v>
+      </c>
+      <c r="C10" s="2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>0.4</v>
+      </c>
+      <c r="C11" s="2">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C12" s="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="C13">
+        <v>130</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="C14">
+        <v>130</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="C15">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>0.51</v>
+      </c>
+      <c r="C16">
+        <v>150</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="C17" s="1">
+        <v>170</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>0.51</v>
+      </c>
+      <c r="C18" s="2">
+        <v>250</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>0.54</v>
+      </c>
+      <c r="C19" s="2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="2">
+        <v>200</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>0.88</v>
+      </c>
+      <c r="C21">
+        <v>150</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>0.52</v>
+      </c>
+      <c r="C22">
+        <v>150</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>